<commit_message>
Replace DataDictionary.xlsx added 71 individuals
</commit_message>
<xml_diff>
--- a/MetadataSchema/DataDictionary.xlsx
+++ b/MetadataSchema/DataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cphillips/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekraus/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CEB8B9-A9E1-BA4B-931A-B498B3961961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0E73E-5306-8F48-AFAD-7F4BDC106EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="580" windowWidth="34560" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="227">
   <si>
     <t>code_system_id</t>
   </si>
@@ -135,27 +135,15 @@
     <t>Data Enclave</t>
   </si>
   <si>
-    <t>Use of cryptographic methods to restrict access and execution to trusted parties and code within a dedicated execution environment</t>
-  </si>
-  <si>
     <t>DataRequester</t>
   </si>
   <si>
     <t>Data Requester</t>
   </si>
   <si>
-    <t>DataSteeringCommittee</t>
-  </si>
-  <si>
-    <t>Data Steering Committee</t>
-  </si>
-  <si>
     <t>DeidentificationMethod</t>
   </si>
   <si>
-    <t>Deidentification Method</t>
-  </si>
-  <si>
     <t>LimitedDataSet</t>
   </si>
   <si>
@@ -165,30 +153,12 @@
     <t>Link</t>
   </si>
   <si>
-    <t>A study in which data from different sources are "linked". Usually used to compile epidemiological data.</t>
-  </si>
-  <si>
-    <t>SafeHarbor</t>
-  </si>
-  <si>
-    <t>Safe Harbor</t>
-  </si>
-  <si>
     <t>Sign</t>
   </si>
   <si>
     <t>Signing a document or agreement</t>
   </si>
   <si>
-    <t>StudySite</t>
-  </si>
-  <si>
-    <t>Study Site</t>
-  </si>
-  <si>
-    <t>NCIt:C15424</t>
-  </si>
-  <si>
     <t>dpv#ResearchAndDevelopment</t>
   </si>
   <si>
@@ -240,13 +210,7 @@
     <t>Is a</t>
   </si>
   <si>
-    <t>An individual who requests access to information that is not the participant</t>
-  </si>
-  <si>
     <t xml:space="preserve">A process to remove the identifiers or any informaiton that could directly identify an individual from a dataset to mitigate privacy risks to that participant </t>
-  </si>
-  <si>
-    <t>A provision granting protection from liability or penalty if certain conditions are met</t>
   </si>
   <si>
     <t xml:space="preserve">Source </t>
@@ -407,35 +371,633 @@
     <t>https://www.w3.org/ns/odrl/2/ODRL22.rdf</t>
   </si>
   <si>
-    <t xml:space="preserve">A location where a research study is conducted </t>
-  </si>
-  <si>
-    <t>https://www.lawinsider.com/dictionary/study-site</t>
-  </si>
-  <si>
     <t>https://www.hhs.gov/hipaa/for-professionals/privacy/special-topics/de-identification/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">The activity or purpose for which the hirer wishes to use the venue </t>
-  </si>
-  <si>
-    <t>https://www.smu.edu/provost/university-decision-support/data-governance/information/steering-committee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A group of individuals who determine the direction and outcome of  data decisions  </t>
-  </si>
-  <si>
-    <t>A set of information about a participant that excludes direct identifiers that are specified in the Privacy Rule.</t>
-  </si>
-  <si>
     <t>https://www.ucihealth.org/-/media/files/pdf/compliance/faqs/research-privacy-faqs.pdf</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Anonymize</t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Classify</t>
+  </si>
+  <si>
+    <t>Collect</t>
+  </si>
+  <si>
+    <t>CommercialSale</t>
+  </si>
+  <si>
+    <t>CompleteTraining</t>
+  </si>
+  <si>
+    <t>Deidentify</t>
+  </si>
+  <si>
+    <t>ObtainApproval</t>
+  </si>
+  <si>
+    <t>ObtainConsent</t>
+  </si>
+  <si>
+    <t>Perform</t>
+  </si>
+  <si>
+    <t>Reidentify</t>
+  </si>
+  <si>
+    <t>RequestAccess</t>
+  </si>
+  <si>
+    <t>ResearchUse</t>
+  </si>
+  <si>
+    <t>MakeDetermination</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deidentify </t>
+  </si>
+  <si>
+    <t>CerficationOrganization</t>
+  </si>
+  <si>
+    <t>An organization that grants or approves certifications or certificates. Includes Certificates of Confidentiality.</t>
+  </si>
+  <si>
+    <t>An individual who requests access to a dataset that is not the participant</t>
+  </si>
+  <si>
+    <t>MinorParticipant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refers to children or persons who have not attained the legal age for consent to treatments or procedures involved in the research, under the applicable law of the jurisdiction in which the research will be conducted (45 CFR 46.402(a)). https://www.hhs.gov/ohrp/regulations-and-policy/guidance/faq/children-research/index.html </t>
+  </si>
+  <si>
+    <t>DataCoordinatingCenter</t>
+  </si>
+  <si>
+    <t>DataProvider</t>
+  </si>
+  <si>
+    <t>Institutions/organizations/researchers that collect data from patients or study participants or that collect administrative data; they may also be the party to submit the data to a repository for sharing</t>
+  </si>
+  <si>
+    <t>DataRepository</t>
+  </si>
+  <si>
+    <t>GovernmentOrganization</t>
+  </si>
+  <si>
+    <t>IRB</t>
+  </si>
+  <si>
+    <t>Guardian</t>
+  </si>
+  <si>
+    <t>PrincipalInvestigatory</t>
+  </si>
+  <si>
+    <t>The investigator with the overall responsibility for the design, conduct, and reporting of the research, and must assure both the protocol and the research team’s actions are compliant with law, regulation, and NIH policy, even when certain aspects of the research are delegated to other investigators. (This definition is cited in Policies 3014-102, 3014-106, and 3014-300)</t>
+  </si>
+  <si>
+    <t>PrivacyBoard</t>
+  </si>
+  <si>
+    <t>ReviewCommittee</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual who is or becomes a participant in research, either as a recipient of the test article or as a control. A subject may be either a healthy human or a patient. https://policymanual.nih.gov/3014-001#C </t>
+  </si>
+  <si>
+    <t>DataAccessCommittee</t>
+  </si>
+  <si>
+    <t>DisclosureReviewBody</t>
+  </si>
+  <si>
+    <t>Policy Type</t>
+  </si>
+  <si>
+    <t>Agreement</t>
+  </si>
+  <si>
+    <t>Certification</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>IRBDocumentation</t>
+  </si>
+  <si>
+    <t>PrivacyBoardDocumentation</t>
+  </si>
+  <si>
+    <t>Law (regulations and statutes)</t>
+  </si>
+  <si>
+    <t>Determination</t>
+  </si>
+  <si>
+    <t>A Policy that grants the assignee a Rule over an Asset from an assigner [ODRL]</t>
+  </si>
+  <si>
+    <t>the process of earning an official document, or the act of providing an official document, as proof that something has happened or been done. [Cambridge University Press] Includes NIH Institutional Certification and other Certifications of Confidentiality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A legally binding agreement between parties that includes the exchange of funds https://docs.oasis-open.org/ubl/cs01-UBL-2.3/UBL-2.3.html#T-CONTRACT </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents generated by or with an IRB including protocols, letters, and decisions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outcome of a legal decision or ruling [LegalRuleML] http://docs.oasis-open.org/legalruleml/legalruleml-core-spec/v1.0/legalruleml-core-spec-v1.0.html Includes a letter of determination that documents an IRB decision on the status of research. (HHS) </t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>VirtualEnvironment</t>
+  </si>
+  <si>
+    <t>LinkageMethod</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>AccessPath</t>
+  </si>
+  <si>
+    <t>ConsentRequirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consent </t>
+  </si>
+  <si>
+    <r>
+      <t>The IRB-approved written record that is in compliance with </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45 CFR 46</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> and as applicable, </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>21 CFR 50 Subparts B and D</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and is used to demonstrate the consent by a subject/Legally Authorized Representative to participate in research. (This definition is cited in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Policy 3014-301</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Commercial Sale</t>
+  </si>
+  <si>
+    <t>Complete Training</t>
+  </si>
+  <si>
+    <t>Make Determination</t>
+  </si>
+  <si>
+    <t>Obtain Approval</t>
+  </si>
+  <si>
+    <t>Obtain Consent</t>
+  </si>
+  <si>
+    <t>Request Access</t>
+  </si>
+  <si>
+    <t>Research Use</t>
+  </si>
+  <si>
+    <t>Cerfication Organization</t>
+  </si>
+  <si>
+    <t>Minor Participant</t>
+  </si>
+  <si>
+    <t>Data Coordinating Center</t>
+  </si>
+  <si>
+    <t>Data Provider</t>
+  </si>
+  <si>
+    <t>Data Repository</t>
+  </si>
+  <si>
+    <t>ControlledAccess</t>
+  </si>
+  <si>
+    <t>Controlled Access</t>
+  </si>
+  <si>
+    <t>Application and eligibility requirements need to be met and approved (e.g., by a data access committee) to gain access. (NIH)
+“Controlled access” and “access controls” refer to measures such as requiring data requesters to verify their identity and the appropriateness of their proposed research use to access protected data. (NIH)</t>
+  </si>
+  <si>
+    <t>Making data available to the broader data user community, for example, by submitting the data to a data repository for dissemination [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t>Working with data for secondary research or other analytical purposes [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t>A set of information about a participant that excludes direct identifiers that are specified in the HIPAA Privacy Rule.</t>
+  </si>
+  <si>
+    <t>To obtain verifiable consent to perform the requested action in relation to the Asset. [ODRL]</t>
+  </si>
+  <si>
+    <t>To obtain verifiable approval to perform the requested action in relation to the Asset.</t>
+  </si>
+  <si>
+    <t>To transfer the ownership of the Asset in perpetuity. [ODRL]</t>
+  </si>
+  <si>
+    <t>To anonymize all or parts of the Asset. [ODRL]</t>
+  </si>
+  <si>
+    <t>SecondaryLink</t>
+  </si>
+  <si>
+    <t>Secondary Link</t>
+  </si>
+  <si>
+    <t>To link a dataset for a secondary purpose distinct from the primary intended and approved purpose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To review materials applicable to an asset such as documents, forms, applications, or protocols. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An institutional review board (IRB) is the institutional entity charged with providing ethical and regulatory oversight of research involving human subjects, typically at the site of the research study. </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(NIH) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>An Institutional Review Board is an appropriately constituted group that has been formally designated to review and monitor biomedical research involving human subjects. An IRB has the authority to approve, require modifications in (to secure approval), or disapprove research. This group review serves an important role in the protection of the rights and welfare of human research subjects</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. FDA)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>An individual who is authorized under applicable State or local law to consent on behalf of a child to general medical care. (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45 CFR 46.402(e)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (This definition is cited in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Policy 3014-402.) Inclusive of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> A child’s biological or adoptive parent. (</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>45 CFR 46.402(d)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) (This definition is cited in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Policy 3014-402</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0B2338"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">A physical location or virtual system where data is stored, managed, and organized for further use. </t>
+  </si>
+  <si>
+    <t>Academic and commercial data management and study oversight organizations, including contract research organizations, whose responsibilities include providing some or all the following services: study administration, financial management, protocol administration, data management, stakeholder communication and coordination, quality assurance, site monitoring, safety, regulatory, document management, post-study management, and close-out activities [NIDDK - https://www.niddk.nih.gov/-/media/Files/Research-Funding/Process/NIDDK-Guidance_DCC-Management-of-CCAs_Final_Version-1,-d-,1_OD-Approved_External-Website.pdf ]</t>
+  </si>
+  <si>
+    <t>To complete training</t>
+  </si>
+  <si>
+    <t>To acquire data from a data repository or other data sharing system [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t>To provide permission to perform data lifecycle activities, including collecting, linking, sharing, accessing, or using the data  [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t>To organize data by relevant categories so that it may be used and protected more efficiently [DAMA-DMBOK]</t>
+  </si>
+  <si>
+    <t>To obtain data from participants for research, clinical, or administrative purposes [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To remove identifiying information. De-identified patient data is patient information that has had personally identifiable information (PII; e.g. a person’s name, email address, or social security number), including protected health information (PHI; e.g. medical history, test results, and insurance information) removed. This is normally performed when sharing the data from a registry or clinical study to prevent a participant from being directly or indirectly identified. (NIH) </t>
+  </si>
+  <si>
+    <t>To combine information from a variety of data sources for the same individual. (AHRQ) Synonymous with record linkage. [NICHD ODSS]</t>
+  </si>
+  <si>
+    <t>ODRL</t>
+  </si>
+  <si>
+    <t>To reach a decision or draw conclusions for the purpose of data analysis</t>
+  </si>
+  <si>
+    <t>To sell for commercial purposes [derived from ODRL definition for CommercialUse]</t>
+  </si>
+  <si>
+    <t>The activity or purpose for which the hirer wishes to use the asset</t>
+  </si>
+  <si>
+    <t>approvedParty</t>
+  </si>
+  <si>
+    <t>approvingParty</t>
+  </si>
+  <si>
+    <t>assignee</t>
+  </si>
+  <si>
+    <t>assigner</t>
+  </si>
+  <si>
+    <t>consentedParty</t>
+  </si>
+  <si>
+    <t>consentingParty</t>
+  </si>
+  <si>
+    <t>contractedParty</t>
+  </si>
+  <si>
+    <t>contractingParty</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>approved Party</t>
+  </si>
+  <si>
+    <t>approving Party</t>
+  </si>
+  <si>
+    <t>consented Party</t>
+  </si>
+  <si>
+    <t>consenting Party</t>
+  </si>
+  <si>
+    <t>contracted Party</t>
+  </si>
+  <si>
+    <t>contracting Party</t>
+  </si>
+  <si>
+    <t>The party receiving action (e.g., receiving consent)</t>
+  </si>
+  <si>
+    <t>The party granting or performing and action (e.g., granting consent)</t>
+  </si>
+  <si>
+    <t>The party providing approval on an asset</t>
+  </si>
+  <si>
+    <t>The party receiving approval on an asset</t>
+  </si>
+  <si>
+    <t>The party receiving consent on an asset</t>
+  </si>
+  <si>
+    <t>The party granting consent on an asset</t>
+  </si>
+  <si>
+    <t>The party granting contractual terms regarding an asset</t>
+  </si>
+  <si>
+    <t>The party receiving and subject to contractual terms regarding an asset</t>
+  </si>
+  <si>
+    <t>To attribute information to de-identified data in order to identify the individual to whom the de-identified data relate [NIST]</t>
+  </si>
+  <si>
+    <t>To request access to a dataset or virtual environment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An international, federal, state, tribal, or local government organization. Inclusive of departments or divisions within a larger government organization. </t>
+  </si>
+  <si>
+    <t>A document which establishes who is permitted to use and receive data, and the permitted uses and disclosures of such information by the recipient. (HHS modified)  An executed agreement between a data provider and a data recipient that specifies the terms under which the data can be used. [NIST]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Privacy Board is a review body that may be established to act upon requests for a waiver or an alteration of the Authorization requirement under the Privacy Rule for uses and disclosures of PHI for a particular research study. A Privacy Board may waive or alter all or part of the Authorization requirements for a specified research project or protocol. A covered entity may use and disclose PHI, without an Authorization, or with an altered Authorization, if it receives the proper documentation of approval of such alteration or waiver from a Privacy Board. [NIH] https://privacyruleandresearch.nih.gov/privacy_boards_hipaa_privacy_rule.asp#:~:text=A%20Privacy%20Board%20is%20a,for%20a%20particular%20research%20study. </t>
+  </si>
+  <si>
+    <t>A group of individuals convened to review research or data related materials and provide approvals and issue determinations on data linkage, sharing, use, and access</t>
+  </si>
+  <si>
+    <t>The dataset that would be access and linked by the data requester to generate a linked dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documents generated by or with a Privacy Board including protocols, letters, and decisions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Process </t>
+  </si>
+  <si>
+    <t>Law</t>
+  </si>
+  <si>
+    <t>SafeHarborMethod</t>
+  </si>
+  <si>
+    <t>Safe Harbor Method</t>
+  </si>
+  <si>
+    <t>A method for deidentification by removal of 18 elements of protected health information defined by the HIPAA Privacy Rule.</t>
+  </si>
+  <si>
+    <t>A secure network through which confidential data, such as identifiable information from census data, can be stored and disseminated. In a virtual data enclave a researcher can access the data from their own computer but cannot download or remove it from the remote server. Higher security data can be accessed through a physical data enclave where a researcher is required to access the data from a monitored room where the data is stored on non-network computers. (NNLM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,6 +1072,48 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0B2338"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0B2338"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -550,7 +1154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -604,7 +1208,44 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -915,7 +1556,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+    <sheetView zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
@@ -948,23 +1589,23 @@
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -972,26 +1613,26 @@
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1015,10 +1656,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="38" x14ac:dyDescent="0.2">
@@ -1028,50 +1669,50 @@
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1110,7 +1751,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>23</v>
@@ -1118,44 +1759,44 @@
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1189,221 +1830,1036 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043D92F7-6FBF-F04C-882C-4B5933BBA611}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F72"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="161" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="51.83203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="73.1640625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="29" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="14" t="s">
+      <c r="C1" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="F1" s="28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>151</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="35" t="s">
+        <v>191</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="30" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>192</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="30" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>193</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D27" s="30" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="30" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D30" s="30" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="D31" s="30" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C33" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="36" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="B48" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="30" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B49" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A50" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A51" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A53" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" s="30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="A54" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="30" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A55" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="30" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A57" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="C57" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A58" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B58" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A60" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A61" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B61" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="33" t="s">
+        <v>222</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="22"/>
+    </row>
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="34"/>
+    </row>
+    <row r="65" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A65" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="C66" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="34"/>
+    </row>
+    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B67" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="15" t="s">
+      <c r="C67" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="E67" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B68" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C68" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A69" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A70" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B70" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C70" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E70" s="29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B71" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F8" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="15" t="s">
+      <c r="C71" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="F12" t="s">
-        <v>98</v>
+      <c r="D71" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="F71" s="29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A72" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="B72" s="29" t="s">
+        <v>224</v>
+      </c>
+      <c r="C72" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="F72" s="29" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F72">
+    <sortCondition ref="C2:C72"/>
+    <sortCondition ref="A2:A72"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="D52" r:id="rId1" display="https://policymanual.nih.gov/3014-001" xr:uid="{03904C53-2335-924E-A385-EB45B50774BF}"/>
+    <hyperlink ref="D59" r:id="rId2" display="https://docs.oasis-open.org/ubl/cs01-UBL-2.3/UBL-2.3.html" xr:uid="{D3CBA20A-9FE8-0044-A7F1-5F68E3436FBE}"/>
+    <hyperlink ref="D60" r:id="rId3" display="https://www.hhs.gov/hipaa/for-professionals/special-topics/emergency-preparedness/data-use-agreement/index.html" xr:uid="{22C1694F-BAA6-554E-BF26-3221B5D6CB3F}"/>
+    <hyperlink ref="D61" r:id="rId4" display="http://docs.oasis-open.org/legalruleml/legalruleml-core-spec/v1.0/legalruleml-core-spec-v1.0.html" xr:uid="{529CC82C-ED26-FA42-BA07-8A1E64686153}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1512,18 +2968,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1724,18 +3180,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1D1DE8-59A4-49D8-BC34-7047ABA6FCC9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD07A8D5-741A-4761-ADD0-98DCD30EB05B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD07A8D5-741A-4761-ADD0-98DCD30EB05B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C1D1DE8-59A4-49D8-BC34-7047ABA6FCC9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Replace DataDictionary.xlsx editted for clarity and completion
</commit_message>
<xml_diff>
--- a/MetadataSchema/DataDictionary.xlsx
+++ b/MetadataSchema/DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekraus/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0E73E-5306-8F48-AFAD-7F4BDC106EE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3891FBC-235A-8442-9177-3FC54474D998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="760" windowWidth="34560" windowHeight="19680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1740" windowWidth="34560" windowHeight="19680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="242">
   <si>
     <t>code_system_id</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>LimitedDataSet</t>
-  </si>
-  <si>
-    <t>Limited Data Set</t>
   </si>
   <si>
     <t>Link</t>
@@ -473,9 +470,6 @@
     <t>Guardian</t>
   </si>
   <si>
-    <t>PrincipalInvestigatory</t>
-  </si>
-  <si>
     <t>The investigator with the overall responsibility for the design, conduct, and reporting of the research, and must assure both the protocol and the research team’s actions are compliant with law, regulation, and NIH policy, even when certain aspects of the research are delegated to other investigators. (This definition is cited in Policies 3014-102, 3014-106, and 3014-300)</t>
   </si>
   <si>
@@ -537,9 +531,6 @@
   </si>
   <si>
     <t>Product</t>
-  </si>
-  <si>
-    <t>Purpose</t>
   </si>
   <si>
     <t>VirtualEnvironment</t>
@@ -991,6 +982,60 @@
   </si>
   <si>
     <t>A secure network through which confidential data, such as identifiable information from census data, can be stored and disseminated. In a virtual data enclave a researcher can access the data from their own computer but cannot download or remove it from the remote server. Higher security data can be accessed through a physical data enclave where a researcher is required to access the data from a monitored room where the data is stored on non-network computers. (NNLM)</t>
+  </si>
+  <si>
+    <t>DeidentifiedDataset</t>
+  </si>
+  <si>
+    <t>Deidentified Dataset</t>
+  </si>
+  <si>
+    <t>Limited Dataset</t>
+  </si>
+  <si>
+    <t>A set of information about a participant that excludes all direct and indirect identifiers that are specified in the HIPAA Privacy Rule and has undergone expert determination or meets Safe Harbor guidelines.</t>
+  </si>
+  <si>
+    <t>PurposeOfUse</t>
+  </si>
+  <si>
+    <t>Purpose of Use</t>
+  </si>
+  <si>
+    <t>The method used for linkage. Inclusive of PPRL and non-PPRL methods.</t>
+  </si>
+  <si>
+    <t>PrincipalInvestigator</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>Privacy Board</t>
+  </si>
+  <si>
+    <t>Review Committee</t>
+  </si>
+  <si>
+    <t>Disclosure Review Body</t>
+  </si>
+  <si>
+    <t>Government Organization</t>
+  </si>
+  <si>
+    <t>Access Path</t>
+  </si>
+  <si>
+    <t>Consent Requirement</t>
+  </si>
+  <si>
+    <t>Deidentification Method</t>
+  </si>
+  <si>
+    <t>Linkage Method</t>
+  </si>
+  <si>
+    <t>Virtual Environment</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1208,42 +1253,33 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1589,23 +1625,23 @@
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>62</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -1613,26 +1649,26 @@
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1656,10 +1692,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="38" x14ac:dyDescent="0.2">
@@ -1669,50 +1705,50 @@
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="20" t="s">
         <v>73</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
         <v>75</v>
-      </c>
-      <c r="B7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="B8" s="20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
         <v>79</v>
-      </c>
-      <c r="B9" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="20" t="s">
         <v>81</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1751,7 +1787,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>23</v>
@@ -1759,44 +1795,44 @@
     </row>
     <row r="2" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="15" t="s">
         <v>48</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1830,1023 +1866,1039 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043D92F7-6FBF-F04C-882C-4B5933BBA611}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="29" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" style="29" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" style="29" customWidth="1"/>
-    <col min="4" max="4" width="73.1640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="29" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="29"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="73.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="28" t="s">
-        <v>58</v>
+      <c r="F1" s="27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B3" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D2" s="23" t="s">
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="26" t="s">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" t="s">
+        <v>147</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="23" t="s">
         <v>170</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B4" s="29" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="30" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="30" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="30" t="s">
+    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="29" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
-        <v>93</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="29" t="s">
+      <c r="B25" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C27" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="29" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>237</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>238</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>241</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>151</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="B41" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" s="29" t="s">
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B42" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="21"/>
+    </row>
+    <row r="43" spans="1:6" ht="128" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>114</v>
+      </c>
+      <c r="B45" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="21"/>
+    </row>
+    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" t="s">
         <v>154</v>
       </c>
-      <c r="C16" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="30" t="s">
+      <c r="C51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53" t="s">
+        <v>232</v>
+      </c>
+      <c r="C53" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="144" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" t="s">
+        <v>233</v>
+      </c>
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="15" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="F23" s="31" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>199</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" s="30" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="35" t="s">
-        <v>191</v>
-      </c>
-      <c r="B25" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="C25" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B26" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="C26" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D26" s="30" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="B27" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="C27" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D27" s="30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>201</v>
-      </c>
-      <c r="C28" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D28" s="30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" s="30" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>203</v>
-      </c>
-      <c r="C30" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D30" s="30" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B31" s="35" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" s="35" t="s">
-        <v>198</v>
-      </c>
-      <c r="D31" s="30" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="35" t="s">
+    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A57" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="A58" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="22" t="s">
         <v>145</v>
-      </c>
-      <c r="B32" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="B33" s="35" t="s">
-        <v>146</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B35" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="B36" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B37" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A38" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="B38" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="30" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="21"/>
-    </row>
-    <row r="43" spans="1:6" ht="128" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" s="30" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="C44" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" s="32" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="36" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B46" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C46" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B47" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="21"/>
-    </row>
-    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="B48" s="29" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" s="29" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="112" x14ac:dyDescent="0.2">
-      <c r="A50" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="C51" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D51" s="30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="80" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>119</v>
-      </c>
-      <c r="C53" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="144" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>121</v>
-      </c>
-      <c r="C54" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D54" s="30" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C55" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="30" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C56" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A57" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="B57" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="C57" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="64" x14ac:dyDescent="0.2">
-      <c r="A58" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="B58" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="C58" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="C59" s="29" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>125</v>
       </c>
       <c r="D59" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="C60" s="29" t="s">
-        <v>127</v>
+        <v>49</v>
+      </c>
+      <c r="C60" t="s">
+        <v>125</v>
       </c>
       <c r="D60" s="21" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A61" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="B61" s="33" t="s">
-        <v>134</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>127</v>
+      <c r="A61" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" t="s">
+        <v>125</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="33" t="s">
+      <c r="A62" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" t="s">
+        <v>125</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="B63" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="B62" s="33" t="s">
-        <v>131</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D62" s="22" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="33" t="s">
+      <c r="C63" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="22"/>
+    </row>
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>125</v>
+      </c>
+      <c r="D64" s="30"/>
+    </row>
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A65" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C66" t="s">
+        <v>125</v>
+      </c>
+      <c r="D66" s="30"/>
+    </row>
+    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" t="s">
+        <v>29</v>
+      </c>
+      <c r="C68" t="s">
+        <v>41</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>158</v>
+      </c>
+      <c r="B69" t="s">
+        <v>159</v>
+      </c>
+      <c r="C69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" t="s">
+        <v>226</v>
+      </c>
+      <c r="C71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>220</v>
+      </c>
+      <c r="B72" t="s">
+        <v>221</v>
+      </c>
+      <c r="C72" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" s="15" t="s">
         <v>222</v>
       </c>
-      <c r="B63" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C63" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" s="22"/>
-    </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B64" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="C64" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" s="34"/>
-    </row>
-    <row r="65" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A65" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="B65" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="C65" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" s="22" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A66" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="B66" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="C66" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="D66" s="34"/>
-    </row>
-    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A67" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B67" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C68" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="30" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="80" x14ac:dyDescent="0.2">
-      <c r="A69" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="B69" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="C69" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="30" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="96" x14ac:dyDescent="0.2">
-      <c r="A70" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="30" t="s">
-        <v>226</v>
-      </c>
-      <c r="E70" s="29" t="s">
+      <c r="F72" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>224</v>
+      </c>
+      <c r="B73" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A71" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B71" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C71" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="F71" s="29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A72" s="29" t="s">
-        <v>223</v>
-      </c>
-      <c r="B72" s="29" t="s">
-        <v>224</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>225</v>
-      </c>
-      <c r="F72" s="29" t="s">
-        <v>59</v>
+      <c r="D73" s="15" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>